<commit_message>
UPDT: Fix metadata templates including INS questionnaire hierarchy
</commit_message>
<xml_diff>
--- a/example/NHANES-2017-2018/SDDs/SDD-NHANES-2017-2018-DEMO.xlsx
+++ b/example/NHANES-2017-2018/SDDs/SDD-NHANES-2017-2018-DEMO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="InfoSheet" sheetId="1" state="visible" r:id="rId3"/>
@@ -1676,8 +1676,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15914,8 +15914,8 @@
   </sheetPr>
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add comment and webdocuments to NHANES instruments
</commit_message>
<xml_diff>
--- a/example/NHANES-2017-2018/SDDs/SDD-NHANES-2017-2018-DEMO.xlsx
+++ b/example/NHANES-2017-2018/SDDs/SDD-NHANES-2017-2018-DEMO.xlsx
@@ -8,13 +8,13 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="InfoSheet" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Prefixes" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Mapping Process" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Timeline" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="New Concepts" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="Codebook" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="Dictionary Mapping" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="InfoSheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Prefixes" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Mapping Process" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Timeline" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="New Concepts" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Codebook" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Dictionary Mapping" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +28,7 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Unknown Author</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="A13" authorId="0">
@@ -36,8 +36,10 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">======
 ID#AAAAO6m9JfE
@@ -51,8 +53,10 @@
         <r>
           <rPr>
             <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">======
 ID#AAAAO6m9JfA
@@ -1087,7 +1091,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1148,11 +1152,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1435,11 +1434,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1451,7 +1450,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1479,11 +1478,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1563,124 +1562,18 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.85"/>
   </cols>
@@ -2791,7 +2684,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2801,7 +2694,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -3879,7 +3772,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3889,7 +3782,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -4969,7 +4862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4979,7 +4872,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -6075,7 +5968,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6085,7 +5978,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.48"/>
@@ -14333,7 +14226,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -14343,7 +14236,7 @@
       <selection pane="topLeft" activeCell="D105" activeCellId="0" sqref="D105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="61"/>
@@ -15908,7 +15801,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -15918,7 +15811,7 @@
       <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.5"/>

</xml_diff>